<commit_message>
replace 10 files of p5 with those in vitas
</commit_message>
<xml_diff>
--- a/dataset_2022/benchmark2022.xlsx
+++ b/dataset_2022/benchmark2022.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2078" uniqueCount="1266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="1266">
   <si>
     <t xml:space="preserve">B081K3R8HJ</t>
   </si>
@@ -4547,8 +4547,8 @@
   </sheetPr>
   <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A90" colorId="64" zoomScale="97" zoomScaleNormal="97" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B110" activeCellId="0" sqref="B110"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="97" zoomScaleNormal="97" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P101" activeCellId="0" sqref="P101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62890625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10732,7 +10732,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>1086</v>
       </c>
@@ -10803,7 +10803,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>1100</v>
       </c>
@@ -10871,7 +10871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>1113</v>
       </c>
@@ -10942,7 +10942,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="126.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>1126</v>
       </c>
@@ -11013,7 +11013,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>1136</v>
       </c>
@@ -11032,9 +11032,8 @@
       <c r="F92" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="G92" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G92" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="H92" s="0" t="s">
         <v>1139</v>
@@ -11048,9 +11047,8 @@
       <c r="K92" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="L92" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="L92" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="M92" s="0" t="s">
         <v>1142</v>
@@ -11086,7 +11084,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>1150</v>
       </c>
@@ -11105,9 +11103,8 @@
       <c r="F93" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="G93" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G93" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="H93" s="0" t="s">
         <v>1153</v>
@@ -11121,9 +11118,8 @@
       <c r="K93" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="L93" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="L93" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="M93" s="0" t="s">
         <v>1155</v>
@@ -11159,7 +11155,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>1163</v>
       </c>
@@ -11178,9 +11174,8 @@
       <c r="F94" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="G94" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G94" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="H94" s="0" t="s">
         <v>1166</v>
@@ -11194,9 +11189,8 @@
       <c r="K94" s="0" t="s">
         <v>1168</v>
       </c>
-      <c r="L94" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="L94" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="M94" s="0" t="s">
         <v>1169</v>
@@ -11232,7 +11226,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>1177</v>
       </c>
@@ -11251,9 +11245,8 @@
       <c r="F95" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="G95" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G95" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="H95" s="0" t="s">
         <v>1180</v>
@@ -11267,9 +11260,8 @@
       <c r="K95" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="L95" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="L95" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="M95" s="0" t="s">
         <v>1182</v>
@@ -11305,7 +11297,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>1190</v>
       </c>
@@ -11324,9 +11316,8 @@
       <c r="F96" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="G96" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G96" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="H96" s="0" t="s">
         <v>1193</v>
@@ -11340,9 +11331,8 @@
       <c r="K96" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="L96" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="L96" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="M96" s="0" t="s">
         <v>1195</v>
@@ -11378,7 +11368,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>1203</v>
       </c>
@@ -11397,9 +11387,8 @@
       <c r="F97" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="G97" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G97" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="H97" s="0" t="s">
         <v>1206</v>
@@ -11413,9 +11402,8 @@
       <c r="K97" s="0" t="s">
         <v>557</v>
       </c>
-      <c r="L97" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="L97" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="M97" s="0" t="s">
         <v>1208</v>
@@ -11451,7 +11439,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>1216</v>
       </c>
@@ -11470,9 +11458,8 @@
       <c r="F98" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="G98" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G98" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="H98" s="0" t="s">
         <v>1218</v>
@@ -11486,9 +11473,8 @@
       <c r="K98" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="L98" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="L98" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="M98" s="0" t="s">
         <v>1220</v>
@@ -11524,7 +11510,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>1227</v>
       </c>
@@ -11543,9 +11529,8 @@
       <c r="F99" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="G99" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G99" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="H99" s="0" t="s">
         <v>1230</v>
@@ -11559,9 +11544,8 @@
       <c r="K99" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="L99" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="L99" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="M99" s="0" t="s">
         <v>1232</v>
@@ -11597,7 +11581,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>1240</v>
       </c>
@@ -11616,9 +11600,8 @@
       <c r="F100" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="G100" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G100" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="H100" s="0" t="s">
         <v>1243</v>
@@ -11632,9 +11615,8 @@
       <c r="K100" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="L100" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="L100" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="M100" s="0" t="s">
         <v>1245</v>
@@ -11670,7 +11652,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>1253</v>
       </c>
@@ -11689,9 +11671,8 @@
       <c r="F101" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="G101" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G101" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="H101" s="0" t="s">
         <v>1256</v>
@@ -11705,9 +11686,8 @@
       <c r="K101" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="L101" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="L101" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="M101" s="0" t="s">
         <v>1258</v>

</xml_diff>

<commit_message>
change permission to bool
</commit_message>
<xml_diff>
--- a/dataset_2022/benchmark2022.xlsx
+++ b/dataset_2022/benchmark2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IoT\4-GPT4_Vitas\GPT4_vitas\dataset_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB8DACE-0630-4602-9568-CD09AA552DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B73985-497A-4EC6-949A-B3A4703BFFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4391,6 +4391,7 @@
       <b/>
       <sz val="11"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -4801,7 +4802,7 @@
   <dimension ref="A1:W101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14" x14ac:dyDescent="0.25"/>

</xml_diff>